<commit_message>
added env example and updated deploy guide
</commit_message>
<xml_diff>
--- a/deploy-guide.xlsx
+++ b/deploy-guide.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Setting" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Deploying Step" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Settings" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Deploying Steps" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="167">
   <si>
     <t xml:space="preserve">Settings</t>
   </si>
@@ -119,9 +119,15 @@
     <t xml:space="preserve">0x458E674dd77A950B08F0962168BA105e814Cd2Cd</t>
   </si>
   <si>
+    <t xml:space="preserve">Owner public key of marketplace contract</t>
+  </si>
+  <si>
     <t xml:space="preserve">PRIVATE_KEY</t>
   </si>
   <si>
+    <t xml:space="preserve">Owner private key of marketplace contract</t>
+  </si>
+  <si>
     <t xml:space="preserve">RPC_URL</t>
   </si>
   <si>
@@ -134,6 +140,9 @@
     <t xml:space="preserve">CONTRACT_ADDRESS</t>
   </si>
   <si>
+    <t xml:space="preserve">Depoyed marketplace contract address</t>
+  </si>
+  <si>
     <t xml:space="preserve">HOST</t>
   </si>
   <si>
@@ -191,7 +200,7 @@
     <t xml:space="preserve">Developer fee</t>
   </si>
   <si>
-    <t xml:space="preserve">Deploying and Launching Step</t>
+    <t xml:space="preserve">Deploying and Launching Steps</t>
   </si>
   <si>
     <t xml:space="preserve">#</t>
@@ -266,25 +275,31 @@
     <t xml:space="preserve">node -v</t>
   </si>
   <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check npm version</t>
   </si>
   <si>
     <t xml:space="preserve">npm -v</t>
   </si>
   <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Install yarn</t>
   </si>
   <si>
     <t xml:space="preserve">npm install --global yarn</t>
   </si>
   <si>
-    <t xml:space="preserve">9</t>
+    <t xml:space="preserve">11</t>
   </si>
   <si>
     <t xml:space="preserve">Go to “Hardhat” directory of project</t>
   </si>
   <si>
-    <t xml:space="preserve">10</t>
+    <t xml:space="preserve">12</t>
   </si>
   <si>
     <t xml:space="preserve">Update hardhat config info</t>
@@ -293,7 +308,7 @@
     <t xml:space="preserve">Add private key of marketplace contract owner - #72 in “hardhat.config.js”</t>
   </si>
   <si>
-    <t xml:space="preserve">11</t>
+    <t xml:space="preserve">13</t>
   </si>
   <si>
     <t xml:space="preserve">Install node modules</t>
@@ -302,7 +317,7 @@
     <t xml:space="preserve">yarn install</t>
   </si>
   <si>
-    <t xml:space="preserve">12</t>
+    <t xml:space="preserve">14</t>
   </si>
   <si>
     <t xml:space="preserve">Check if hardhat was installed</t>
@@ -311,7 +326,7 @@
     <t xml:space="preserve">npx hardhat</t>
   </si>
   <si>
-    <t xml:space="preserve">13</t>
+    <t xml:space="preserve">15</t>
   </si>
   <si>
     <t xml:space="preserve">Clean old files compiled</t>
@@ -320,7 +335,7 @@
     <t xml:space="preserve">npx hardhat clean</t>
   </si>
   <si>
-    <t xml:space="preserve">14</t>
+    <t xml:space="preserve">16</t>
   </si>
   <si>
     <t xml:space="preserve">Deploy contract to mainnet</t>
@@ -329,7 +344,7 @@
     <t xml:space="preserve">npx hardhat run scripts/deploy-mainnet.js --network mainnet</t>
   </si>
   <si>
-    <t xml:space="preserve">15</t>
+    <t xml:space="preserve">17</t>
   </si>
   <si>
     <t xml:space="preserve">Verify if you want</t>
@@ -338,7 +353,7 @@
     <t xml:space="preserve">npx hardhat verify --network mainnet “CorsacNFTFactory address” “CorsacERC721 address” “CorsacERC1155 address”</t>
   </si>
   <si>
-    <t xml:space="preserve">16</t>
+    <t xml:space="preserve">18</t>
   </si>
   <si>
     <t xml:space="preserve">Morails</t>
@@ -347,19 +362,19 @@
     <t xml:space="preserve">Create account on morails.io</t>
   </si>
   <si>
-    <t xml:space="preserve">17</t>
+    <t xml:space="preserve">19</t>
   </si>
   <si>
     <t xml:space="preserve">Upgrade moralis account plan</t>
   </si>
   <si>
-    <t xml:space="preserve">18</t>
+    <t xml:space="preserve">20</t>
   </si>
   <si>
     <t xml:space="preserve">Create new moralis server</t>
   </si>
   <si>
-    <t xml:space="preserve">19</t>
+    <t xml:space="preserve">21</t>
   </si>
   <si>
     <t xml:space="preserve">Config moralis server</t>
@@ -368,7 +383,7 @@
     <t xml:space="preserve">Please refer old moralis server</t>
   </si>
   <si>
-    <t xml:space="preserve">20</t>
+    <t xml:space="preserve">22</t>
   </si>
   <si>
     <t xml:space="preserve">Sync “ListedOnSale” event from contract</t>
@@ -377,25 +392,37 @@
     <t xml:space="preserve">Will plain and config in detail via telegram or anydesk</t>
   </si>
   <si>
-    <t xml:space="preserve">21</t>
+    <t xml:space="preserve">23</t>
   </si>
   <si>
     <t xml:space="preserve">Prepare ubuntu 20.04 LTS server</t>
   </si>
   <si>
-    <t xml:space="preserve">22</t>
+    <t xml:space="preserve">24</t>
   </si>
   <si>
     <t xml:space="preserve">Prepare domain/base url for Back-end APIs</t>
   </si>
   <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please refer step#3-#9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check yarn version</t>
   </si>
   <si>
     <t xml:space="preserve">yarn –version</t>
   </si>
   <si>
-    <t xml:space="preserve">23</t>
+    <t xml:space="preserve">28</t>
   </si>
   <si>
     <t xml:space="preserve">Go to /var/www/ and then make new directory</t>
@@ -404,28 +431,34 @@
     <t xml:space="preserve">mkdir “Domain for back-end”</t>
   </si>
   <si>
-    <t xml:space="preserve">24</t>
+    <t xml:space="preserve">29</t>
   </si>
   <si>
     <t xml:space="preserve">Clone source from git</t>
   </si>
   <si>
-    <t xml:space="preserve">25</t>
+    <t xml:space="preserve">30</t>
   </si>
   <si>
     <t xml:space="preserve">Go to back-end directory</t>
   </si>
   <si>
-    <t xml:space="preserve">26</t>
+    <t xml:space="preserve">31</t>
   </si>
   <si>
     <t xml:space="preserve">Edit .env file</t>
   </si>
   <si>
-    <t xml:space="preserve">Please refer “Setting” tab on this document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
+    <t xml:space="preserve">Change .env.example to .env and then set the values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please refer “Settings” tab on this document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33</t>
   </si>
   <si>
     <t xml:space="preserve">Install nginx server</t>
@@ -434,7 +467,7 @@
     <t xml:space="preserve">Please refer this link - https://www.digitalocean.com/community/tutorials/how-to-install-nginx-on-ubuntu-20-04</t>
   </si>
   <si>
-    <t xml:space="preserve">28</t>
+    <t xml:space="preserve">34</t>
   </si>
   <si>
     <t xml:space="preserve">Config nginx server for back-end</t>
@@ -443,7 +476,7 @@
     <t xml:space="preserve">Make new file “domain for back-end”.conf and edit it as old back-end - /etc/nginx/sites-available/apinftv2.corsac.io.conf</t>
   </si>
   <si>
-    <t xml:space="preserve">29</t>
+    <t xml:space="preserve">35</t>
   </si>
   <si>
     <t xml:space="preserve">Install pm2 (process manager for Node.js applications) for manage back-end</t>
@@ -452,13 +485,13 @@
     <t xml:space="preserve">npm install pm2@latest -g</t>
   </si>
   <si>
-    <t xml:space="preserve">30</t>
+    <t xml:space="preserve">36</t>
   </si>
   <si>
     <t xml:space="preserve">Install node modules for back-end</t>
   </si>
   <si>
-    <t xml:space="preserve">31</t>
+    <t xml:space="preserve">37</t>
   </si>
   <si>
     <t xml:space="preserve">Run back-end</t>
@@ -467,25 +500,25 @@
     <t xml:space="preserve">pm2 start app.js –watch</t>
   </si>
   <si>
-    <t xml:space="preserve">32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose server – Netlify or IPFS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33</t>
+    <t xml:space="preserve">38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose server - Netlify or IPFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39</t>
   </si>
   <si>
     <t xml:space="preserve">Connect front-end from github</t>
   </si>
   <si>
-    <t xml:space="preserve">34</t>
+    <t xml:space="preserve">40</t>
   </si>
   <si>
     <t xml:space="preserve">Config setting for build front-end</t>
   </si>
   <si>
-    <t xml:space="preserve">35</t>
+    <t xml:space="preserve">41</t>
   </si>
   <si>
     <t xml:space="preserve">Build front-end project</t>
@@ -501,7 +534,7 @@
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -525,6 +558,13 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -536,6 +576,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -599,7 +644,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -616,12 +661,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -632,7 +677,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -640,11 +685,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -664,12 +713,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -677,10 +726,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -764,7 +817,7 @@
   <dimension ref="B2:G31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -819,12 +872,12 @@
       <c r="F5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -842,7 +895,7 @@
       <c r="G6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="7" t="s">
@@ -854,7 +907,7 @@
       <c r="G7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7" t="s">
@@ -868,7 +921,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="7" t="s">
@@ -882,7 +935,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
@@ -896,7 +949,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="7" t="s">
@@ -908,7 +961,7 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="7" t="s">
@@ -924,7 +977,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="7" t="s">
         <v>25</v>
       </c>
@@ -938,7 +991,7 @@
       <c r="G13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -953,64 +1006,70 @@
       <c r="F14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="6"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="G15" s="10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="6"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="6"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="6"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="6"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F19" s="6" t="n">
         <v>27017</v>
@@ -1020,36 +1079,38 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="6"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="6"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G21" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="G21" s="6" t="n">
+        <v>2083</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="6"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="6"/>
       <c r="D22" s="7" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>27</v>
@@ -1058,29 +1119,29 @@
       <c r="G22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="6" t="s">
-        <v>45</v>
+      <c r="B23" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="11" t="s">
-        <v>35</v>
+        <v>50</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="6"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6" t="n">
@@ -1088,11 +1149,11 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="6"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F25" s="6" t="n">
         <v>20000000000</v>
@@ -1102,39 +1163,39 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="6"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="6"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="F27" s="11" t="n">
         <v>0.025</v>
       </c>
-      <c r="G27" s="10" t="n">
+      <c r="G27" s="11" t="n">
         <v>0.01</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="6"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F28" s="6" t="n">
         <v>0</v>
@@ -1144,11 +1205,11 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="6"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F29" s="6" t="n">
         <v>0</v>
@@ -1212,562 +1273,593 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:E53"/>
+  <dimension ref="B2:E55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="3.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="3.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="26.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="62.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="12" width="118.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="6" style="12" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1022" style="14" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="3.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="3.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="26.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="62.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="13" width="118.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="6" style="13" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1022" style="15" width="11.54"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="B2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="17" t="s">
+      <c r="B5" s="17" t="s">
         <v>60</v>
       </c>
+      <c r="C5" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="19"/>
+      <c r="B6" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>66</v>
+      <c r="B7" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="19" t="s">
+      <c r="B8" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="21"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="21"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="21"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="21"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" s="21"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E29" s="21"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="22" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="19"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="20"/>
+      <c r="D35" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="21"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" s="20"/>
+      <c r="D38" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="20"/>
+      <c r="D39" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="20"/>
+      <c r="D40" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41" s="20"/>
+      <c r="D41" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="E41" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="E23" s="19"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="E24" s="19"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" s="19"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="E28" s="19"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="E29" s="19"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="E34" s="19"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="20"/>
+      <c r="D42" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E43" s="21"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="E44" s="21"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="20"/>
+      <c r="D45" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="E45" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="E39" s="19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E41" s="19"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="E42" s="19"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="E44" s="19"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="18"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
+      <c r="B46" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C46" s="20"/>
+      <c r="D46" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E46" s="21"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="18"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="18"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="18"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="18"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="18"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="18"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="18"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="19"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="19"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="B2:E4"/>
     <mergeCell ref="C6:C22"/>
     <mergeCell ref="D8:D12"/>
     <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C28:C40"/>
-    <mergeCell ref="C41:C44"/>
+    <mergeCell ref="C28:C42"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="C43:C46"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1" display="git clone https://github.com/blkdot/corsacv2_nft_marketplace.git"/>
-    <hyperlink ref="E33" r:id="rId2" display="git clone https://github.com/blkdot/corsacv2_nft_marketplace.git"/>
-    <hyperlink ref="E36" r:id="rId3" display="Please refer this link - https://www.digitalocean.com/community/tutorials/how-to-install-nginx-on-ubuntu-20-04"/>
+    <hyperlink ref="E34" r:id="rId2" display="git clone https://github.com/blkdot/corsacv2_nft_marketplace.git"/>
+    <hyperlink ref="E38" r:id="rId3" display="Please refer this link - https://www.digitalocean.com/community/tutorials/how-to-install-nginx-on-ubuntu-20-04"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
updated deploy script and guide
</commit_message>
<xml_diff>
--- a/deploy-guide.xlsx
+++ b/deploy-guide.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="176">
   <si>
     <t xml:space="preserve">Settings</t>
   </si>
@@ -290,16 +290,43 @@
     <t xml:space="preserve">Install yarn</t>
   </si>
   <si>
-    <t xml:space="preserve">npm install --global yarn</t>
+    <t xml:space="preserve">curl -sS https://dl.yarnpkg.com/debian/pubkey.gpg | sudo apt-key add -</t>
   </si>
   <si>
     <t xml:space="preserve">11</t>
   </si>
   <si>
+    <t xml:space="preserve">echo "deb https://dl.yarnpkg.com/debian/ stable main" | sudo tee /etc/apt/sources.list.d/yarn.list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo apt update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo apt install yarn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check yarn version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yarn -v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
     <t xml:space="preserve">Go to “Hardhat” directory of project</t>
   </si>
   <si>
-    <t xml:space="preserve">12</t>
+    <t xml:space="preserve">16</t>
   </si>
   <si>
     <t xml:space="preserve">Update hardhat config info</t>
@@ -308,7 +335,7 @@
     <t xml:space="preserve">Add private key of marketplace contract owner - #72 in “hardhat.config.js”</t>
   </si>
   <si>
-    <t xml:space="preserve">13</t>
+    <t xml:space="preserve">17</t>
   </si>
   <si>
     <t xml:space="preserve">Install node modules</t>
@@ -317,7 +344,7 @@
     <t xml:space="preserve">yarn install</t>
   </si>
   <si>
-    <t xml:space="preserve">14</t>
+    <t xml:space="preserve">18</t>
   </si>
   <si>
     <t xml:space="preserve">Check if hardhat was installed</t>
@@ -326,7 +353,7 @@
     <t xml:space="preserve">npx hardhat</t>
   </si>
   <si>
-    <t xml:space="preserve">15</t>
+    <t xml:space="preserve">19</t>
   </si>
   <si>
     <t xml:space="preserve">Clean old files compiled</t>
@@ -335,7 +362,7 @@
     <t xml:space="preserve">npx hardhat clean</t>
   </si>
   <si>
-    <t xml:space="preserve">16</t>
+    <t xml:space="preserve">20</t>
   </si>
   <si>
     <t xml:space="preserve">Deploy contract to mainnet</t>
@@ -344,7 +371,7 @@
     <t xml:space="preserve">npx hardhat run scripts/deploy-mainnet.js --network mainnet</t>
   </si>
   <si>
-    <t xml:space="preserve">17</t>
+    <t xml:space="preserve">21</t>
   </si>
   <si>
     <t xml:space="preserve">Verify if you want</t>
@@ -353,7 +380,7 @@
     <t xml:space="preserve">npx hardhat verify --network mainnet “CorsacNFTFactory address” “CorsacERC721 address” “CorsacERC1155 address”</t>
   </si>
   <si>
-    <t xml:space="preserve">18</t>
+    <t xml:space="preserve">22</t>
   </si>
   <si>
     <t xml:space="preserve">Morails</t>
@@ -362,19 +389,19 @@
     <t xml:space="preserve">Create account on morails.io</t>
   </si>
   <si>
-    <t xml:space="preserve">19</t>
+    <t xml:space="preserve">23</t>
   </si>
   <si>
     <t xml:space="preserve">Upgrade moralis account plan</t>
   </si>
   <si>
-    <t xml:space="preserve">20</t>
+    <t xml:space="preserve">24</t>
   </si>
   <si>
     <t xml:space="preserve">Create new moralis server</t>
   </si>
   <si>
-    <t xml:space="preserve">21</t>
+    <t xml:space="preserve">25</t>
   </si>
   <si>
     <t xml:space="preserve">Config moralis server</t>
@@ -383,7 +410,7 @@
     <t xml:space="preserve">Please refer old moralis server</t>
   </si>
   <si>
-    <t xml:space="preserve">22</t>
+    <t xml:space="preserve">26</t>
   </si>
   <si>
     <t xml:space="preserve">Sync “ListedOnSale” event from contract</t>
@@ -392,37 +419,37 @@
     <t xml:space="preserve">Will plain and config in detail via telegram or anydesk</t>
   </si>
   <si>
-    <t xml:space="preserve">23</t>
+    <t xml:space="preserve">27</t>
   </si>
   <si>
     <t xml:space="preserve">Prepare ubuntu 20.04 LTS server</t>
   </si>
   <si>
-    <t xml:space="preserve">24</t>
+    <t xml:space="preserve">28</t>
   </si>
   <si>
     <t xml:space="preserve">Prepare domain/base url for Back-end APIs</t>
   </si>
   <si>
-    <t xml:space="preserve">25</t>
+    <t xml:space="preserve">29</t>
   </si>
   <si>
     <t xml:space="preserve">Please refer step#3-#9</t>
   </si>
   <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check yarn version</t>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please refer step#10-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31</t>
   </si>
   <si>
     <t xml:space="preserve">yarn –version</t>
   </si>
   <si>
-    <t xml:space="preserve">28</t>
+    <t xml:space="preserve">32</t>
   </si>
   <si>
     <t xml:space="preserve">Go to /var/www/ and then make new directory</t>
@@ -431,19 +458,19 @@
     <t xml:space="preserve">mkdir “Domain for back-end”</t>
   </si>
   <si>
-    <t xml:space="preserve">29</t>
+    <t xml:space="preserve">33</t>
   </si>
   <si>
     <t xml:space="preserve">Clone source from git</t>
   </si>
   <si>
-    <t xml:space="preserve">30</t>
+    <t xml:space="preserve">34</t>
   </si>
   <si>
     <t xml:space="preserve">Go to back-end directory</t>
   </si>
   <si>
-    <t xml:space="preserve">31</t>
+    <t xml:space="preserve">35</t>
   </si>
   <si>
     <t xml:space="preserve">Edit .env file</t>
@@ -452,13 +479,13 @@
     <t xml:space="preserve">Change .env.example to .env and then set the values.</t>
   </si>
   <si>
-    <t xml:space="preserve">32</t>
+    <t xml:space="preserve">36</t>
   </si>
   <si>
     <t xml:space="preserve">Please refer “Settings” tab on this document</t>
   </si>
   <si>
-    <t xml:space="preserve">33</t>
+    <t xml:space="preserve">37</t>
   </si>
   <si>
     <t xml:space="preserve">Install nginx server</t>
@@ -467,7 +494,7 @@
     <t xml:space="preserve">Please refer this link - https://www.digitalocean.com/community/tutorials/how-to-install-nginx-on-ubuntu-20-04</t>
   </si>
   <si>
-    <t xml:space="preserve">34</t>
+    <t xml:space="preserve">38</t>
   </si>
   <si>
     <t xml:space="preserve">Config nginx server for back-end</t>
@@ -476,7 +503,7 @@
     <t xml:space="preserve">Make new file “domain for back-end”.conf and edit it as old back-end - /etc/nginx/sites-available/apinftv2.corsac.io.conf</t>
   </si>
   <si>
-    <t xml:space="preserve">35</t>
+    <t xml:space="preserve">39</t>
   </si>
   <si>
     <t xml:space="preserve">Install pm2 (process manager for Node.js applications) for manage back-end</t>
@@ -485,13 +512,13 @@
     <t xml:space="preserve">npm install pm2@latest -g</t>
   </si>
   <si>
-    <t xml:space="preserve">36</t>
+    <t xml:space="preserve">40</t>
   </si>
   <si>
     <t xml:space="preserve">Install node modules for back-end</t>
   </si>
   <si>
-    <t xml:space="preserve">37</t>
+    <t xml:space="preserve">41</t>
   </si>
   <si>
     <t xml:space="preserve">Run back-end</t>
@@ -500,25 +527,25 @@
     <t xml:space="preserve">pm2 start app.js –watch</t>
   </si>
   <si>
-    <t xml:space="preserve">38</t>
+    <t xml:space="preserve">42</t>
   </si>
   <si>
     <t xml:space="preserve">Choose server - Netlify or IPFS</t>
   </si>
   <si>
-    <t xml:space="preserve">39</t>
+    <t xml:space="preserve">43</t>
   </si>
   <si>
     <t xml:space="preserve">Connect front-end from github</t>
   </si>
   <si>
-    <t xml:space="preserve">40</t>
+    <t xml:space="preserve">44</t>
   </si>
   <si>
     <t xml:space="preserve">Config setting for build front-end</t>
   </si>
   <si>
-    <t xml:space="preserve">41</t>
+    <t xml:space="preserve">45</t>
   </si>
   <si>
     <t xml:space="preserve">Build front-end project</t>
@@ -685,10 +712,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -734,6 +757,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1018,7 +1045,7 @@
         <v>33</v>
       </c>
       <c r="F15" s="6"/>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1131,8 +1158,8 @@
       <c r="E23" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="12" t="s">
+      <c r="F23" s="10"/>
+      <c r="G23" s="11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1183,10 +1210,10 @@
       <c r="E27" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="11" t="n">
+      <c r="F27" s="10" t="n">
         <v>0.025</v>
       </c>
-      <c r="G27" s="11" t="n">
+      <c r="G27" s="10" t="n">
         <v>0.01</v>
       </c>
     </row>
@@ -1273,593 +1300,636 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:E55"/>
+  <dimension ref="B2:E59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="3.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="3.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="26.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="62.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="13" width="118.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="6" style="13" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1022" style="15" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="3.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="3.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="26.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="62.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="12" width="118.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="6" style="12" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1022" style="14" width="11.54"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="21"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="21" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="20" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21" t="s">
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21" t="s">
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21" t="s">
+      <c r="C13" s="19"/>
+      <c r="D13" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="20" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="21" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="20" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21" t="s">
+      <c r="C15" s="19"/>
+      <c r="D15" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="20" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="E16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21" t="s">
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="21" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="18" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="19" t="s">
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="C19" s="19"/>
+      <c r="D19" s="20" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="19" t="s">
+      <c r="E19" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="C20" s="19"/>
+      <c r="D20" s="20" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="19" t="s">
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21" t="s">
+      <c r="C21" s="19"/>
+      <c r="D21" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E21" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="19" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21" t="s">
+      <c r="C22" s="19"/>
+      <c r="D22" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E22" s="20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="19" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="21" t="s">
+      <c r="C23" s="19"/>
+      <c r="D23" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E23" s="20" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="19" t="s">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C24" s="19"/>
+      <c r="D24" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="E24" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="E23" s="21"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="19" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="21" t="s">
+      <c r="C25" s="19"/>
+      <c r="D25" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="E24" s="21"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="19" t="s">
+      <c r="E25" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="21"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="19" t="s">
+      <c r="C26" s="19"/>
+      <c r="D26" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21" t="s">
+      <c r="E26" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E26" s="21" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="18" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="19" t="s">
+      <c r="C27" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="18" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="19" t="s">
+      <c r="C28" s="19"/>
+      <c r="D28" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="E28" s="20"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" s="20"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="E28" s="21"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="E29" s="21"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="21" t="s">
+      <c r="D32" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="20"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E30" s="21" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="21" t="s">
+      <c r="E34" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="E31" s="21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="E34" s="22" t="s">
+      <c r="E35" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" s="19"/>
+      <c r="D38" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="E38" s="21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="E35" s="21"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="E38" s="22" t="s">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="18" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="19" t="s">
+      <c r="C39" s="19"/>
+      <c r="D39" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="21" t="s">
+      <c r="E39" s="20"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="E39" s="21" t="s">
+      <c r="C40" s="19"/>
+      <c r="D40" s="20" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="19" t="s">
+      <c r="E40" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="21" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="C41" s="19"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="19" t="s">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="E41" s="21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="19" t="s">
+      <c r="E42" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="C42" s="20"/>
-      <c r="D42" s="21" t="s">
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="E42" s="21" t="s">
+      <c r="C43" s="19"/>
+      <c r="D43" s="20" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="19" t="s">
+      <c r="E43" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="C43" s="20" t="s">
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" s="19"/>
+      <c r="D44" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="19"/>
+      <c r="D45" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="C46" s="19"/>
+      <c r="D46" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C47" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="E43" s="21"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="E44" s="21"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="E45" s="21" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="C46" s="20"/>
-      <c r="D46" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="E46" s="21"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="19"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
+      <c r="D47" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="E47" s="20"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="19"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
+      <c r="B48" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="C48" s="19"/>
+      <c r="D48" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="E48" s="20"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="19"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
+      <c r="B49" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C49" s="19"/>
+      <c r="D49" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="19"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
+      <c r="B50" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" s="19"/>
+      <c r="D50" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="E50" s="20"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="19"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="19"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="19"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="19"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="19"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="18"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="18"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="18"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="18"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B2:E4"/>
-    <mergeCell ref="C6:C22"/>
+    <mergeCell ref="C6:C26"/>
     <mergeCell ref="D8:D12"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C28:C42"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="C32:C46"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="C47:C50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1" display="git clone https://github.com/blkdot/corsacv2_nft_marketplace.git"/>
-    <hyperlink ref="E34" r:id="rId2" display="git clone https://github.com/blkdot/corsacv2_nft_marketplace.git"/>
-    <hyperlink ref="E38" r:id="rId3" display="Please refer this link - https://www.digitalocean.com/community/tutorials/how-to-install-nginx-on-ubuntu-20-04"/>
+    <hyperlink ref="E38" r:id="rId2" display="git clone https://github.com/blkdot/corsacv2_nft_marketplace.git"/>
+    <hyperlink ref="E42" r:id="rId3" display="Please refer this link - https://www.digitalocean.com/community/tutorials/how-to-install-nginx-on-ubuntu-20-04"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
updated guide and fixed bug for admin user
</commit_message>
<xml_diff>
--- a/deploy-guide.xlsx
+++ b/deploy-guide.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="210">
   <si>
     <t xml:space="preserve">Settings</t>
   </si>
@@ -545,7 +545,33 @@
     <t xml:space="preserve">43</t>
   </si>
   <si>
-    <t xml:space="preserve">Install pm2 (process manager for Node.js applications) for manage back-end</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Install pm2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">for manage back-end 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(process manager for Node.js applications)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">yarn global add pm2</t>
@@ -581,40 +607,50 @@
     <t xml:space="preserve">Check back-end is running</t>
   </si>
   <si>
+    <t xml:space="preserve">Add BNB as default payment on mongoDB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show databases;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use market_db;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db.payments.find({}).pretty();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db.payments.insert({id: 0, type: 0, address: '', title: 'Binance', symbol: 'BNB', decimals: 18, allowed: 1});</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.exit</t>
+  </si>
+  <si>
     <t xml:space="preserve">48</t>
   </si>
   <si>
-    <t xml:space="preserve">Add BNB as default payment on mongoDB</t>
+    <t xml:space="preserve">Add admin account info on mongoDB 
+(It should be an owner of marketplace on mainnet.)</t>
   </si>
   <si>
     <t xml:space="preserve">49</t>
   </si>
   <si>
-    <t xml:space="preserve">show databases;</t>
-  </si>
-  <si>
     <t xml:space="preserve">50</t>
   </si>
   <si>
-    <t xml:space="preserve">use market_db;</t>
-  </si>
-  <si>
     <t xml:space="preserve">51</t>
   </si>
   <si>
-    <t xml:space="preserve">db.payments.find({}).pretty();</t>
+    <t xml:space="preserve">db.users.find({}).pretty();</t>
   </si>
   <si>
     <t xml:space="preserve">52</t>
   </si>
   <si>
-    <t xml:space="preserve">db.payments.insert({id: 0, type: 0, address: '', title: 'Binance', symbol: 'BNB', decimals: 18, allowed: 1});</t>
+    <t xml:space="preserve">db.users.insert({walletAddr: "admin wallet address", name: "admin", avatar: "", banner: "", about: "", twitter: "", youtube: "", instagram: "", created_at: 1654287617, isAdmin: 1});</t>
   </si>
   <si>
     <t xml:space="preserve">53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.exit</t>
   </si>
   <si>
     <t xml:space="preserve">54</t>
@@ -654,7 +690,7 @@
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -721,6 +757,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -810,7 +851,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -905,6 +946,10 @@
     </xf>
     <xf numFmtId="167" fontId="9" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1510,20 +1555,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:F71"/>
+  <dimension ref="B2:F79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G66" activeCellId="0" sqref="G66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="26.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="62.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="13" width="119"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="6" style="13" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="45.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="13" width="153.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="13" width="10.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="7" style="13" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1023" style="15" width="11.57"/>
   </cols>
   <sheetData>
@@ -2169,12 +2215,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="19" t="s">
         <v>173</v>
       </c>
       <c r="C48" s="20"/>
-      <c r="D48" s="21" t="s">
+      <c r="D48" s="24" t="s">
         <v>174</v>
       </c>
       <c r="E48" s="21" t="s">
@@ -2245,12 +2291,10 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="19" t="s">
-        <v>186</v>
-      </c>
+      <c r="B53" s="19"/>
       <c r="C53" s="20"/>
       <c r="D53" s="21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E53" s="21" t="s">
         <v>172</v>
@@ -2260,173 +2304,209 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="19" t="s">
-        <v>188</v>
-      </c>
+      <c r="B54" s="19"/>
       <c r="C54" s="20"/>
       <c r="D54" s="21"/>
       <c r="E54" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F54" s="21" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="19" t="s">
-        <v>190</v>
-      </c>
+      <c r="B55" s="19"/>
       <c r="C55" s="20"/>
       <c r="D55" s="21"/>
       <c r="E55" s="21" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F55" s="21" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="19" t="s">
-        <v>192</v>
-      </c>
+      <c r="B56" s="19"/>
       <c r="C56" s="20"/>
       <c r="D56" s="21"/>
       <c r="E56" s="21" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F56" s="21" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="19" t="s">
-        <v>194</v>
-      </c>
+      <c r="B57" s="19"/>
       <c r="C57" s="20"/>
       <c r="D57" s="21"/>
       <c r="E57" s="21" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F57" s="21" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="19" t="s">
-        <v>196</v>
-      </c>
+      <c r="B58" s="19"/>
       <c r="C58" s="20"/>
       <c r="D58" s="21"/>
       <c r="E58" s="21" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="F58" s="21" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="C59" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D59" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="E59" s="21"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21" t="s">
+        <v>191</v>
+      </c>
       <c r="F59" s="21" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="19" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C60" s="20"/>
-      <c r="D60" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
+      <c r="D60" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="19" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C61" s="20"/>
-      <c r="D61" s="21" t="s">
-        <v>204</v>
-      </c>
+      <c r="D61" s="24"/>
       <c r="E61" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="F61" s="21"/>
+        <v>187</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="19" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C62" s="20"/>
-      <c r="D62" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F62" s="21" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="19"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
+      <c r="B63" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="C63" s="20"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="F63" s="21" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="19"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
-      <c r="E64" s="21"/>
-      <c r="F64" s="21"/>
+      <c r="B64" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="C64" s="20"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="F64" s="21" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="19"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="21"/>
-      <c r="F65" s="21"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="F65" s="21" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="19"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
+      <c r="B66" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="C66" s="20"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="F66" s="21" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="19"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
+      <c r="B67" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="21" t="s">
+        <v>202</v>
+      </c>
       <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
+      <c r="F67" s="21" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="19"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
+      <c r="B68" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C68" s="20"/>
+      <c r="D68" s="21" t="s">
+        <v>205</v>
+      </c>
       <c r="E68" s="21"/>
       <c r="F68" s="21"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="19"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="21"/>
+      <c r="B69" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C69" s="20"/>
+      <c r="D69" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="E69" s="21" t="s">
+        <v>155</v>
+      </c>
       <c r="F69" s="21"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="19"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
+      <c r="B70" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="C70" s="20"/>
+      <c r="D70" s="21" t="s">
+        <v>209</v>
+      </c>
       <c r="E70" s="21"/>
       <c r="F70" s="21"/>
     </row>
@@ -2437,46 +2517,103 @@
       <c r="E71" s="21"/>
       <c r="F71" s="21"/>
     </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="19"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="19"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="19"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="19"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="19"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="21"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="19"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="21"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="19"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="19"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="21"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="B2:F4"/>
     <mergeCell ref="C6:C26"/>
     <mergeCell ref="D8:D12"/>
     <mergeCell ref="D15:D18"/>
     <mergeCell ref="C27:C31"/>
-    <mergeCell ref="C32:C58"/>
+    <mergeCell ref="C32:C66"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D53:D58"/>
-    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="D53:D59"/>
+    <mergeCell ref="D60:D66"/>
+    <mergeCell ref="C67:C70"/>
   </mergeCells>
-  <conditionalFormatting sqref="D6:F71">
+  <conditionalFormatting sqref="D6:F79">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$F6="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:F71">
+  <conditionalFormatting sqref="D6:F79">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>$F6="Preparing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:F71">
+  <conditionalFormatting sqref="D6:F79">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>$F6="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:F71">
+  <conditionalFormatting sqref="D6:F79">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>$F6="Cancelled"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:F71">
+  <conditionalFormatting sqref="D6:F79">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>$F6="Processing"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F71" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F79" type="list">
       <formula1>"Preparing,Prepared,Processing,Completed,Failed,Cancelled"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>